<commit_message>
Atualização do projeto TDD com uso do Extent Report.
</commit_message>
<xml_diff>
--- a/src/test/resources/Planilha/massaLogin.xlsx
+++ b/src/test/resources/Planilha/massaLogin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonardo.sonoda\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonardo.sonoda\eclipse-workspace\ProjetoHubTDD\src\test\resources\Planilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D538BB5B-86DA-4183-9EED-9521EF0DBABD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFC1FA1-533E-4C9A-8596-9CC1218F1AF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E1CBC9E3-B228-4629-913F-61EC9E25F53B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Senha</t>
   </si>
@@ -45,6 +45,21 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>jorge_jorge</t>
+  </si>
+  <si>
+    <t>123456Senha</t>
+  </si>
+  <si>
+    <t>Cadastrado</t>
+  </si>
+  <si>
+    <t>jorge_egorj</t>
+  </si>
+  <si>
+    <t>UserName Incorreto</t>
   </si>
 </sst>
 </file>
@@ -241,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -258,7 +273,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -268,12 +282,28 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,20 +618,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA372ED0-D6E5-46BE-8AFA-64122AE51875}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -615,99 +645,112 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="11"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="15"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
   </sheetData>

</xml_diff>